<commit_message>
Correction pour génération automatique schémas mapping 32bcb8dbf034944f31112b1c447d440458285f80
</commit_message>
<xml_diff>
--- a/mapping-pn13/ig/StructureDefinition-oncofair-cp-Pharmacist.xlsx
+++ b/mapping-pn13/ig/StructureDefinition-oncofair-cp-Pharmacist.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="129">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-22T14:39:57+00:00</t>
+    <t>2024-04-22T15:15:59+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -252,9 +252,6 @@
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>PROTOCOLE PRESCRIT</t>
   </si>
   <si>
     <t>Extension.id</t>
@@ -981,7 +978,7 @@
         <v>78</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="AL2" t="s" s="2">
         <v>74</v>
@@ -989,10 +986,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1003,25 +1000,25 @@
         <v>75</v>
       </c>
       <c r="G3" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K3" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="H3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="J3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="L3" t="s" s="2">
+      <c r="M3" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="M3" t="s" s="2">
-        <v>84</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1072,37 +1069,37 @@
         <v>74</v>
       </c>
       <c r="AF3" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AG3" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH3" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI3" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="AG3" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI3" t="s" s="2">
+      <c r="AJ3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL3" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="AJ3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL3" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
@@ -1121,16 +1118,16 @@
         <v>74</v>
       </c>
       <c r="K4" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="L4" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="L4" t="s" s="2">
+      <c r="M4" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="M4" t="s" s="2">
+      <c r="N4" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="N4" t="s" s="2">
-        <v>93</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -1168,19 +1165,19 @@
         <v>74</v>
       </c>
       <c r="AB4" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AC4" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AC4" t="s" s="2">
+      <c r="AD4" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE4" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="AD4" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE4" t="s" s="2">
+      <c r="AF4" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="AF4" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>75</v>
@@ -1198,18 +1195,18 @@
         <v>74</v>
       </c>
       <c r="AL4" t="s" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>98</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>99</v>
       </c>
       <c r="D5" t="s" s="2">
         <v>74</v>
@@ -1219,7 +1216,7 @@
         <v>75</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>74</v>
@@ -1231,13 +1228,13 @@
         <v>74</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L5" t="s" s="2">
         <v>27</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1288,7 +1285,7 @@
         <v>74</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>75</v>
@@ -1303,7 +1300,7 @@
         <v>78</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AL5" t="s" s="2">
         <v>74</v>
@@ -1311,10 +1308,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>102</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1325,25 +1322,25 @@
         <v>75</v>
       </c>
       <c r="G6" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K6" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="H6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="K6" t="s" s="2">
+      <c r="L6" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>84</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1394,33 +1391,33 @@
         <v>74</v>
       </c>
       <c r="AF6" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI6" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="AG6" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI6" t="s" s="2">
+      <c r="AJ6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK6" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL6" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL6" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>104</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>105</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1443,13 +1440,13 @@
         <v>74</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L7" t="s" s="2">
         <v>27</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1488,19 +1485,19 @@
         <v>74</v>
       </c>
       <c r="AB7" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AC7" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AC7" t="s" s="2">
+      <c r="AD7" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE7" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="AD7" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE7" t="s" s="2">
+      <c r="AF7" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="AF7" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>75</v>
@@ -1523,10 +1520,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>106</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>107</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1534,10 +1531,10 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>74</v>
@@ -1549,16 +1546,16 @@
         <v>74</v>
       </c>
       <c r="K8" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L8" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L8" t="s" s="2">
+      <c r="M8" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="M8" t="s" s="2">
+      <c r="N8" t="s" s="2">
         <v>110</v>
-      </c>
-      <c r="N8" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -1566,7 +1563,7 @@
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S8" t="s" s="2">
         <v>74</v>
@@ -1608,33 +1605,33 @@
         <v>74</v>
       </c>
       <c r="AF8" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AG8" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH8" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL8" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="AG8" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AH8" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL8" t="s" s="2">
-        <v>113</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
@@ -1645,7 +1642,7 @@
         <v>75</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s" s="2">
         <v>74</v>
@@ -1657,13 +1654,13 @@
         <v>74</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L9" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>118</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1714,36 +1711,36 @@
         <v>74</v>
       </c>
       <c r="AF9" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AG9" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH9" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI9" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="AG9" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH9" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI9" t="s" s="2">
+      <c r="AJ9" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="AJ9" t="s" s="2">
-        <v>121</v>
-      </c>
       <c r="AK9" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s" s="2">
         <v>122</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>123</v>
       </c>
       <c r="D10" t="s" s="2">
         <v>74</v>
@@ -1753,7 +1750,7 @@
         <v>75</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>74</v>
@@ -1765,13 +1762,13 @@
         <v>74</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" t="s" s="2">
         <v>27</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1822,7 +1819,7 @@
         <v>74</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>75</v>
@@ -1837,7 +1834,7 @@
         <v>78</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>74</v>
@@ -1845,10 +1842,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -1859,25 +1856,25 @@
         <v>75</v>
       </c>
       <c r="G11" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="H11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="J11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="K11" t="s" s="2">
+      <c r="L11" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="L11" t="s" s="2">
+      <c r="M11" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>84</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1928,33 +1925,33 @@
         <v>74</v>
       </c>
       <c r="AF11" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AG11" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH11" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI11" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="AG11" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH11" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI11" t="s" s="2">
+      <c r="AJ11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL11" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="AJ11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL11" t="s" s="2">
-        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -1977,13 +1974,13 @@
         <v>74</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s" s="2">
         <v>27</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2022,19 +2019,19 @@
         <v>74</v>
       </c>
       <c r="AB12" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="AC12" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="AC12" t="s" s="2">
+      <c r="AD12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE12" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="AD12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE12" t="s" s="2">
+      <c r="AF12" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>75</v>
@@ -2057,10 +2054,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2068,10 +2065,10 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>74</v>
@@ -2083,16 +2080,16 @@
         <v>74</v>
       </c>
       <c r="K13" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L13" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L13" t="s" s="2">
+      <c r="M13" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="M13" t="s" s="2">
+      <c r="N13" t="s" s="2">
         <v>110</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -2100,7 +2097,7 @@
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" t="s" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S13" t="s" s="2">
         <v>74</v>
@@ -2142,33 +2139,33 @@
         <v>74</v>
       </c>
       <c r="AF13" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL13" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="AG13" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL13" t="s" s="2">
-        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2179,7 +2176,7 @@
         <v>75</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>74</v>
@@ -2191,13 +2188,13 @@
         <v>74</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="L14" t="s" s="2">
+      <c r="M14" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>118</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2248,33 +2245,33 @@
         <v>74</v>
       </c>
       <c r="AF14" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AG14" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH14" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI14" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="AG14" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI14" t="s" s="2">
+      <c r="AJ14" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="AJ14" t="s" s="2">
-        <v>121</v>
-      </c>
       <c r="AK14" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -2282,10 +2279,10 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>74</v>
@@ -2297,16 +2294,16 @@
         <v>74</v>
       </c>
       <c r="K15" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L15" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="L15" t="s" s="2">
+      <c r="M15" t="s" s="2">
         <v>109</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>110</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -2356,33 +2353,33 @@
         <v>74</v>
       </c>
       <c r="AF15" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AG15" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH15" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK15" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL15" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="AG15" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AH15" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AK15" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>113</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -2405,13 +2402,13 @@
         <v>74</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L16" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="M16" t="s" s="2">
         <v>117</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>118</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -2462,25 +2459,25 @@
         <v>74</v>
       </c>
       <c r="AF16" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AG16" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH16" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI16" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="AG16" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH16" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI16" t="s" s="2">
+      <c r="AJ16" t="s" s="2">
         <v>120</v>
       </c>
-      <c r="AJ16" t="s" s="2">
-        <v>121</v>
-      </c>
       <c r="AK16" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>